<commit_message>
rename daschland_data.xml into data_daschland.xml
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Material.xlsx
+++ b/data/spreadsheets/Material.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88A9CE3-8858-F34C-A605-A53A5B9D0206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC5E3F-1156-F84B-8BB7-408BFE31095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18840" yWindow="500" windowWidth="42100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,9 +52,6 @@
     <t>xml file used for the import of data on DSP</t>
   </si>
   <si>
-    <t>daschland_data.xml</t>
-  </si>
-  <si>
     <t>DaSCH</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>Authorship Resource</t>
+  </si>
+  <si>
+    <t>data_daschland.xml</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -644,487 +644,487 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
         <v>33</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
         <v>42</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>43</v>
       </c>
-      <c r="C12" t="s">
-        <v>44</v>
-      </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>49</v>
       </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" t="s">
         <v>51</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>52</v>
       </c>
-      <c r="C15" t="s">
-        <v>53</v>
-      </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
         <v>54</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
       <c r="D16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>58</v>
       </c>
-      <c r="C17" t="s">
-        <v>59</v>
-      </c>
       <c r="D17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
-        <v>62</v>
-      </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>64</v>
       </c>
-      <c r="C19" t="s">
-        <v>65</v>
-      </c>
       <c r="D19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>67</v>
       </c>
-      <c r="C20" t="s">
-        <v>68</v>
-      </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move nodegoat files so spreadsheet folder
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Material.xlsx
+++ b/data/spreadsheets/Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC5E3F-1156-F84B-8BB7-408BFE31095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978BC7AB-E218-384E-BFB8-2C755DCF7030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="500" windowWidth="42100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18840" yWindow="620" windowWidth="42100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>Archive.csv</t>
   </si>
   <si>
-    <t>data/nodegoat/</t>
-  </si>
-  <si>
     <t>MAT_003</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>data_daschland.xml</t>
+  </si>
+  <si>
+    <t>data/spreadsheets/</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -687,16 +687,16 @@
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -713,16 +713,16 @@
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -739,16 +739,16 @@
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -765,16 +765,16 @@
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -791,16 +791,16 @@
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -817,16 +817,16 @@
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -843,16 +843,16 @@
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -869,16 +869,16 @@
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -895,16 +895,16 @@
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -921,16 +921,16 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -947,16 +947,16 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -973,16 +973,16 @@
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -999,16 +999,16 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1025,16 +1025,16 @@
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1051,16 +1051,16 @@
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1077,16 +1077,16 @@
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>66</v>
       </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
move nodegoat files so spreadsheet folder (#82)
</commit_message>
<xml_diff>
--- a/data/spreadsheets/Material.xlsx
+++ b/data/spreadsheets/Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC5E3F-1156-F84B-8BB7-408BFE31095D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978BC7AB-E218-384E-BFB8-2C755DCF7030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18840" yWindow="500" windowWidth="42100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18840" yWindow="620" windowWidth="42100" windowHeight="14320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -70,9 +70,6 @@
     <t>Archive.csv</t>
   </si>
   <si>
-    <t>data/nodegoat/</t>
-  </si>
-  <si>
     <t>MAT_003</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>data_daschland.xml</t>
+  </si>
+  <si>
+    <t>data/spreadsheets/</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,7 +633,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -644,7 +644,7 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -670,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -687,16 +687,16 @@
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -713,16 +713,16 @@
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -739,16 +739,16 @@
     </row>
     <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -765,16 +765,16 @@
     </row>
     <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
         <v>26</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -791,16 +791,16 @@
     </row>
     <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -817,16 +817,16 @@
     </row>
     <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
       <c r="D9" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -843,16 +843,16 @@
     </row>
     <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -869,16 +869,16 @@
     </row>
     <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" t="s">
         <v>38</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
-        <v>40</v>
-      </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -895,16 +895,16 @@
     </row>
     <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -921,16 +921,16 @@
     </row>
     <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>45</v>
       </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -947,16 +947,16 @@
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>48</v>
       </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
       <c r="D14" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -973,16 +973,16 @@
     </row>
     <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" t="s">
-        <v>52</v>
-      </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -999,16 +999,16 @@
     </row>
     <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
         <v>53</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
-        <v>55</v>
-      </c>
       <c r="D16" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
@@ -1025,16 +1025,16 @@
     </row>
     <row r="17" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
-        <v>58</v>
-      </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1051,16 +1051,16 @@
     </row>
     <row r="18" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" t="s">
         <v>59</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>61</v>
-      </c>
       <c r="D18" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1077,16 +1077,16 @@
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" t="s">
-        <v>64</v>
-      </c>
       <c r="D19" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1103,16 +1103,16 @@
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
         <v>65</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>66</v>
       </c>
-      <c r="C20" t="s">
-        <v>67</v>
-      </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>

</xml_diff>